<commit_message>
add state change behavior
</commit_message>
<xml_diff>
--- a/lab_2/reflectance_data_analysis.xlsx
+++ b/lab_2/reflectance_data_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aengus Kennedy\Documents\GitHub\ME0134-Aengus-Kennedy\lab_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D83EA67-D58B-4AAF-9204-899A30296385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AEB008C-3DE6-4B65-A75B-0FCA236E6F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,20 +18,12 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$7</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$8:$B$31</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$C$7</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$C$8:$C$31</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$D$7</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$D$8:$D$31</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$E$7</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$E$8:$E$31</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$7</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$8:$C$31</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$D$7</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$D$8:$D$31</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$E$7</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$E$8:$E$31</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$B$7</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$B$8:$B$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>